<commit_message>
Added code and other business case documents
</commit_message>
<xml_diff>
--- a/Documents/Functional Requirements (user stories)/Functional Requirements_User Stories_V2_Team2.xlsx
+++ b/Documents/Functional Requirements (user stories)/Functional Requirements_User Stories_V2_Team2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="157">
   <si>
     <t>Iteration</t>
   </si>
@@ -51,16 +51,19 @@
     <t>Customer</t>
   </si>
   <si>
+    <t>Register to the website</t>
+  </si>
+  <si>
+    <t>Register to the website and Log in to access the features.</t>
+  </si>
+  <si>
+    <t>01.02 Sign in Account</t>
+  </si>
+  <si>
     <t>Login to the website</t>
   </si>
   <si>
-    <t>Login to the website and access the features.</t>
-  </si>
-  <si>
-    <t>01.02 Sign in Account</t>
-  </si>
-  <si>
-    <t>Access the application and use the provided features</t>
+    <t>Log in to the website, Access the application and use the provided features</t>
   </si>
   <si>
     <t>TBD</t>
@@ -1265,10 +1268,10 @@
         <v>10</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="1"/>
@@ -1294,22 +1297,22 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="2"/>
@@ -1341,37 +1344,37 @@
         <v>8</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7" s="26"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G8" s="31"/>
       <c r="H8" s="1"/>
@@ -1397,22 +1400,22 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="32" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G9" s="31"/>
       <c r="H9" s="2"/>
@@ -1444,16 +1447,16 @@
         <v>8</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" s="34" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G10" s="26"/>
       <c r="H10" s="2"/>
@@ -1479,22 +1482,22 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" s="37" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G11" s="31"/>
       <c r="H11" s="2"/>
@@ -1523,19 +1526,19 @@
         <v>7</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G12" s="26"/>
       <c r="H12" s="2"/>
@@ -1564,166 +1567,166 @@
         <v>7</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G13" s="26"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G14" s="31"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G15" s="31"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" s="44" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F16" s="45" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G16" s="46"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="42" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="47" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E17" s="44" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F17" s="45" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G17" s="46"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="42" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" s="44" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F18" s="45" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G18" s="46"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" s="48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E19" s="50" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G19" s="52"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20" s="48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E20" s="50" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F20" s="51" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G20" s="52"/>
     </row>
@@ -1732,19 +1735,19 @@
         <v>7</v>
       </c>
       <c r="B21" s="54" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" s="55" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D21" s="56" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E21" s="57" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F21" s="58" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G21" s="59"/>
     </row>
@@ -1753,59 +1756,59 @@
         <v>7</v>
       </c>
       <c r="B22" s="54" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C22" s="55" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D22" s="56" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E22" s="58" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F22" s="58" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G22" s="59"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="60" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B23" s="48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C23" s="61" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D23" s="62" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E23" s="45" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F23" s="45" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G23" s="46"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="63"/>
       <c r="B24" s="48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C24" s="64" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D24" s="62" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E24" s="44" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F24" s="45" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G24" s="46"/>
     </row>
@@ -1814,464 +1817,464 @@
         <v>7</v>
       </c>
       <c r="B25" s="54" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C25" s="55" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D25" s="56" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E25" s="58" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F25" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G25" s="59"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="60" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B26" s="48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C26" s="64" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D26" s="62" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E26" s="45" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F26" s="45" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G26" s="46"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="65"/>
       <c r="B27" s="48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C27" s="61" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D27" s="62" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E27" s="45" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F27" s="45" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G27" s="46"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="65"/>
       <c r="B28" s="48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C28" s="64" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D28" s="62" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E28" s="45" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F28" s="45" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G28" s="46"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="65"/>
       <c r="B29" s="48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C29" s="64" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D29" s="62" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E29" s="45" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F29" s="45" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G29" s="46"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="65"/>
       <c r="B30" s="48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C30" s="64" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D30" s="62" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E30" s="66" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F30" s="67" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G30" s="68"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="65"/>
       <c r="B31" s="48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C31" s="64" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D31" s="62" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E31" s="67" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F31" s="67" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G31" s="68"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="63"/>
       <c r="B32" s="48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C32" s="64" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D32" s="62" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E32" s="67" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F32" s="67" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G32" s="68"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="69" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B33" s="48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C33" s="64" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D33" s="70" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E33" s="67" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F33" s="67" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G33" s="68"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="65"/>
       <c r="B34" s="48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C34" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="F34" s="67" t="s">
         <v>107</v>
-      </c>
-      <c r="D34" s="70" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="67" t="s">
-        <v>105</v>
-      </c>
-      <c r="F34" s="67" t="s">
-        <v>106</v>
       </c>
       <c r="G34" s="68"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="65"/>
       <c r="B35" s="48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C35" s="71" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D35" s="70" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E35" s="67" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F35" s="67" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G35" s="68"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="65"/>
       <c r="B36" s="48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C36" s="72" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D36" s="70" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E36" s="67" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F36" s="67" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G36" s="68"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="65"/>
       <c r="B37" s="48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C37" s="72" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E37" s="67" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F37" s="67" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G37" s="68"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="65"/>
       <c r="B38" s="73" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C38" s="74" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D38" s="37" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E38" s="67" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F38" s="67" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G38" s="68"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="63"/>
       <c r="B39" s="48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C39" s="74" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D39" s="37" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E39" s="67" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F39" s="67" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G39" s="68"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="69" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B40" s="48" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C40" s="64" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D40" s="37" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E40" s="67" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F40" s="67" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G40" s="68"/>
     </row>
     <row r="41" ht="18.75" customHeight="1">
       <c r="A41" s="65"/>
       <c r="B41" s="48" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C41" s="71" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D41" s="37" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E41" s="67" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F41" s="67" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G41" s="68"/>
     </row>
     <row r="42" ht="21.0" customHeight="1">
       <c r="A42" s="63"/>
       <c r="B42" s="48" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C42" s="71" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D42" s="37" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E42" s="67" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F42" s="67" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G42" s="68"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="69" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B43" s="48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C43" s="71" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D43" s="75" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E43" s="67" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F43" s="67" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G43" s="68"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="65"/>
       <c r="B44" s="48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C44" s="71" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D44" s="75" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E44" s="67" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F44" s="67" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G44" s="68"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="65"/>
       <c r="B45" s="48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C45" s="71" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D45" s="75" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E45" s="67" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F45" s="67" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G45" s="68"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="65"/>
       <c r="B46" s="48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C46" s="71" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D46" s="75" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E46" s="67" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F46" s="67" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G46" s="68"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="65"/>
       <c r="B47" s="48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C47" s="72" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D47" s="75" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E47" s="67" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F47" s="67" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G47" s="68"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="63"/>
       <c r="B48" s="48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C48" s="71" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D48" s="75" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E48" s="67" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F48" s="67" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G48" s="68"/>
     </row>

</xml_diff>